<commit_message>
Teme za CSS predavanja Prezentacija za prvo predavanje iz CSS-a
</commit_message>
<xml_diff>
--- a/general/Raspored casova.xlsx
+++ b/general/Raspored casova.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kurs-front-end\general\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sinisav\Documents\kurs-front-end\general\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="1170" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
   <si>
     <t>Datum</t>
   </si>
@@ -363,6 +363,24 @@
   </si>
   <si>
     <t>25.5.2018</t>
+  </si>
+  <si>
+    <t>Advanced CSS selctors</t>
+  </si>
+  <si>
+    <t>Animation</t>
+  </si>
+  <si>
+    <t>CSS frameworks - Bootstrap</t>
+  </si>
+  <si>
+    <t>Introduction to CSS, box model, selectors</t>
+  </si>
+  <si>
+    <t>CSS - Layouts, responsive design, media queries</t>
+  </si>
+  <si>
+    <t>Sinisa</t>
   </si>
 </sst>
 </file>
@@ -423,7 +441,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +466,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -507,7 +531,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="2" applyFont="1"/>
@@ -518,6 +542,7 @@
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="5"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -803,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1043,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>32</v>
       </c>
@@ -1032,7 +1057,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="7" t="s">
         <v>33</v>
       </c>
@@ -1043,7 +1068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="7" t="s">
         <v>34</v>
       </c>
@@ -1054,7 +1079,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
         <v>35</v>
       </c>
@@ -1065,7 +1090,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>40</v>
       </c>
@@ -1075,8 +1100,14 @@
       <c r="D21" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>41</v>
       </c>
@@ -1086,8 +1117,14 @@
       <c r="D22" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>42</v>
       </c>
@@ -1097,8 +1134,14 @@
       <c r="D23" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F23" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -1111,8 +1154,14 @@
       <c r="D24" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>44</v>
       </c>
@@ -1125,8 +1174,14 @@
       <c r="D25" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="6" t="s">
         <v>45</v>
       </c>
@@ -1137,7 +1192,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6" t="s">
         <v>46</v>
       </c>
@@ -1148,7 +1203,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="7" t="s">
         <v>47</v>
       </c>
@@ -1159,7 +1214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="7" t="s">
         <v>48</v>
       </c>
@@ -1170,7 +1225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>49</v>
       </c>
@@ -1181,7 +1236,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="6" t="s">
         <v>50</v>
       </c>
@@ -1192,7 +1247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="6" t="s">
         <v>51</v>
       </c>

</xml_diff>